<commit_message>
Adding my name to excel file
</commit_message>
<xml_diff>
--- a/Iteration 3/Use Cases.xlsx
+++ b/Iteration 3/Use Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4b95806db7470f0c/Documents/Education/CSI 3471 Software Engineering One/CharMyCourse/ChartMyCourse/Iteration 3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/varunapte/Desktop/softwareDev1/ChartMyCourse/Iteration 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="11_F25DC773A252ABDACC104838F95E47425BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB3BCAF1-7582-4A63-9DFC-CD006941FCF2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CC4A25-70C8-EB46-9449-13BC808B3AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Use Case</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Warren</t>
+  </si>
+  <si>
+    <t>Varun</t>
   </si>
 </sst>
 </file>
@@ -423,16 +426,16 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,27 +443,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -468,27 +477,30 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -496,7 +508,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -504,7 +516,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -512,7 +524,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -520,47 +532,47 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>

</xml_diff>